<commit_message>
Description:     Minor copy edits before distribution to hdf5lib. Tested:  Firefox
</commit_message>
<xml_diff>
--- a/hdf5doc_support/assignments/H5Dread_questions.xlsx
+++ b/hdf5doc_support/assignments/H5Dread_questions.xlsx
@@ -2,21 +2,30 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="18135" windowHeight="6630"/>
+    <workbookView xWindow="120" yWindow="100" windowWidth="16500" windowHeight="16240"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="18">
+  <si>
+    <t>In this section, pretend you are a new user to HDF who is trying to write and read data, and answer these questions with that frame of mind.</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
   <si>
     <t>yes</t>
   </si>
@@ -45,12 +54,6 @@
     <t>Are there terms in the entry that you don't understand?  If yes, please note them in the notes column.</t>
   </si>
   <si>
-    <t>If you were going to use this function is there additional information you would like to know that is not in the entry? If yes, note what that information is.</t>
-  </si>
-  <si>
-    <t>What type of user would use this function? (HDF library developer,  tool or application developer, user reading an HDF dataset) - answer in notes column</t>
-  </si>
-  <si>
     <t>What else should we have asked?</t>
   </si>
   <si>
@@ -63,17 +66,39 @@
     <t>In the first section, answer the questions based on your current knowledge and understanding of HDF5.</t>
   </si>
   <si>
-    <t>Reference Manual Entry: H5open</t>
-  </si>
-  <si>
-    <t>In this section, pretend you are a new user to HDF who is trying to write data, and answer these questions with that frame of mind.</t>
+    <t>If you were going to use this function, is there additional information you would like to know that is not in the entry? If yes, note what that information is.</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>What type of user would use this function? (HDF library developer,  tool or application developer, user reading an HDF dataset) - answer in notes column.</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>Reference Manual Entry: H5</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>read</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>If you were going to use this function, is there additional information you would like to know that is not in the entry? If yes, note what that information is.</t>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -104,6 +129,31 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -141,19 +191,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -167,13 +211,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -461,226 +517,227 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="34.140625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="6.85546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="7.5703125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="2"/>
-    <col min="5" max="5" width="39.42578125" style="2" customWidth="1"/>
-    <col min="6" max="8" width="9.140625" style="2"/>
+    <col min="1" max="1" width="34.1640625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="6.83203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="7.5" style="2" customWidth="1"/>
+    <col min="4" max="4" width="8.83203125" style="2"/>
+    <col min="5" max="5" width="39.5" style="2" customWidth="1"/>
+    <col min="6" max="8" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="30" customHeight="1">
-      <c r="A1" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
+      <c r="A1" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
     </row>
     <row r="2" spans="1:8" ht="18.75" customHeight="1">
-      <c r="A2" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
+      <c r="A2" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="6"/>
-      <c r="B3" s="7" t="s">
+      <c r="A3" s="4"/>
+      <c r="B3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="32.25" customHeight="1">
+      <c r="A4" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="7"/>
+    </row>
+    <row r="5" spans="1:8" ht="30">
+      <c r="A5" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="7"/>
+    </row>
+    <row r="6" spans="1:8" ht="48" customHeight="1">
+      <c r="A6" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="7"/>
+    </row>
+    <row r="7" spans="1:8" ht="42.75" customHeight="1">
+      <c r="A7" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="7"/>
+    </row>
+    <row r="8" spans="1:8" ht="61.5" customHeight="1">
+      <c r="A8" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="7"/>
+    </row>
+    <row r="9" spans="1:8" ht="75" customHeight="1">
+      <c r="A9" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="7"/>
+    </row>
+    <row r="10" spans="1:8" ht="60">
+      <c r="A10" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="7"/>
+    </row>
+    <row r="11" spans="1:8" ht="51" customHeight="1">
+      <c r="A11" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="7"/>
+    </row>
+    <row r="12" spans="1:8" ht="30" customHeight="1">
+      <c r="A12" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="4"/>
+      <c r="B13" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="C13" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="D13" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="37" customHeight="1">
+      <c r="A14" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="10"/>
+    </row>
+    <row r="15" spans="1:8" ht="30">
+      <c r="A15" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="7"/>
+    </row>
+    <row r="16" spans="1:8" ht="30">
+      <c r="A16" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="7"/>
+    </row>
+    <row r="17" spans="1:5" ht="48.75" customHeight="1">
+      <c r="A17" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="7"/>
+    </row>
+    <row r="18" spans="1:5" ht="30">
+      <c r="A18" s="7" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="32.25" customHeight="1">
-      <c r="A4" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-    </row>
-    <row r="5" spans="1:8" ht="45">
-      <c r="A5" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-    </row>
-    <row r="6" spans="1:8" ht="48" customHeight="1">
-      <c r="A6" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-    </row>
-    <row r="7" spans="1:8" ht="42.75" customHeight="1">
-      <c r="A7" s="9" t="s">
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="7"/>
+    </row>
+    <row r="19" spans="1:5" ht="30">
+      <c r="A19" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-    </row>
-    <row r="8" spans="1:8" ht="61.5" customHeight="1">
-      <c r="A8" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-    </row>
-    <row r="9" spans="1:8" ht="75" customHeight="1">
-      <c r="A9" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-    </row>
-    <row r="10" spans="1:8" ht="75">
-      <c r="A10" s="9" t="s">
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="7"/>
+    </row>
+    <row r="20" spans="1:5" ht="77.25" customHeight="1">
+      <c r="A20" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="7"/>
+    </row>
+    <row r="21" spans="1:5" ht="51" customHeight="1">
+      <c r="A21" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-    </row>
-    <row r="11" spans="1:8" ht="51" customHeight="1">
-      <c r="A11" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-    </row>
-    <row r="12" spans="1:8" ht="30" customHeight="1">
-      <c r="A12" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="A13" s="6"/>
-      <c r="B13" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="E13" s="8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="34.5" customHeight="1">
-      <c r="A14" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="8"/>
-    </row>
-    <row r="15" spans="1:8" ht="30">
-      <c r="A15" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-    </row>
-    <row r="16" spans="1:8" ht="45">
-      <c r="A16" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B16" s="10"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-    </row>
-    <row r="17" spans="1:5" ht="48.75" customHeight="1">
-      <c r="A17" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B17" s="10"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-    </row>
-    <row r="18" spans="1:5" ht="45">
-      <c r="A18" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B18" s="10"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-    </row>
-    <row r="19" spans="1:5" ht="45">
-      <c r="A19" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B19" s="10"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-    </row>
-    <row r="20" spans="1:5" ht="77.25" customHeight="1">
-      <c r="A20" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B20" s="10"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
-    </row>
-    <row r="21" spans="1:5" ht="51" customHeight="1">
-      <c r="A21" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B21" s="10"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="10"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -688,31 +745,49 @@
     <mergeCell ref="A12:E12"/>
     <mergeCell ref="A1:E1"/>
   </mergeCells>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>